<commit_message>
Finally got a nice UML
</commit_message>
<xml_diff>
--- a/WorkBot/refactor/data/orders/Hill & Markes/Hill & Markes_Collegetown_2025-07-25.xlsx
+++ b/WorkBot/refactor/data/orders/Hill & Markes/Hill & Markes_Collegetown_2025-07-25.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,39 +451,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>INPSDR0120ITHACABAKERY</t>
+          <t>INPSDR0160ITHACABAKERY</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cup - Hot (12oz)</t>
+          <t>Cup - Hot (16oz)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>62.78</t>
+          <t>70.09</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>62.78</t>
+          <t>140.18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>INPSDR0160ITHACABAKERY</t>
+          <t>JNA26W</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cup - Hot (16oz)</t>
+          <t>Straws - Wrapped</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -493,51 +493,51 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>70.09</t>
+          <t>59.31</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>140.18</t>
+          <t>118.62</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>JNA26W</t>
+          <t>7G084018</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Straws - Wrapped</t>
+          <t>Bag Poly - 8x4x18 LW</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>59.31</t>
+          <t>29.31</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>118.62</t>
+          <t>29.31</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>7G084018</t>
+          <t>INPSDR0200ITHACABAKERY</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bag Poly - 8x4x18 LW</t>
+          <t>Cup - Hot (20oz)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -547,24 +547,24 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>29.31</t>
+          <t>83.13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>29.31</t>
+          <t>83.13</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>INPSDR0200ITHACABAKERY</t>
+          <t>INLSLP17XD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cup - Hot (20oz)</t>
+          <t>Container - Plastic Eclair</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -574,24 +574,24 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>83.13</t>
+          <t>72.89</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>83.13</t>
+          <t>72.89</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>INLSLP17XD</t>
+          <t>KC12SITHACA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Container - Plastic Eclair</t>
+          <t>Cup - Cold (12oz)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -601,24 +601,24 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>72.89</t>
+          <t>87.78</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>72.89</t>
+          <t>87.78</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>KC12SITHACA</t>
+          <t>DUSSK5</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cup - Cold (12oz)</t>
+          <t>Knife - Smart Stock</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -628,37 +628,10 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>87.78</t>
+          <t>42.71</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
-        <is>
-          <t>87.78</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>DUSSK5</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Knife - Smart Stock</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>42.71</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
         <is>
           <t>42.71</t>
         </is>

</xml_diff>